<commit_message>
Update for first May 2024
</commit_message>
<xml_diff>
--- a/Data Source/dimDates.xlsx
+++ b/Data Source/dimDates.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -530,17 +530,32 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2024-04-18</t>
-        </is>
+      <c r="A7" s="2" t="n">
+        <v>45412</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>https://web.archive.org/web/20240430111825/https://www.oryxspioenkop.com/2022/02/attack-on-europe-documenting-equipment.html</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>https://web.archive.org/web/20240430110305/https://www.oryxspioenkop.com/2022/02/attack-on-europe-documenting-ukrainian.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2024-05-01</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
           <t>https://www.oryxspioenkop.com/2022/02/attack-on-europe-documenting-equipment.html</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>https://www.oryxspioenkop.com/2022/02/attack-on-europe-documenting-ukrainian.html</t>
         </is>

</xml_diff>